<commit_message>
v1.02 STILL NEED TO FIGURE OUT HOW TO CYCLE THO
</commit_message>
<xml_diff>
--- a/homies.xlsx
+++ b/homies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilen\Desktop\ANDRES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9331ED-96ED-4ED8-A397-491E306B1915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6205CF9B-5BB8-4356-9651-27C38AA9BC9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{BA09453C-118F-4BA7-BAAB-6338DA55BF77}"/>
+    <workbookView xWindow="4260" yWindow="3315" windowWidth="21600" windowHeight="11385" xr2:uid="{BA09453C-118F-4BA7-BAAB-6338DA55BF77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Dylan</t>
   </si>
@@ -42,19 +42,76 @@
     <t>Haworth</t>
   </si>
   <si>
+    <t>DeChoch</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Guzman</t>
+  </si>
+  <si>
+    <t>Kaydin</t>
+  </si>
+  <si>
+    <t>Brooksher</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Menjivar</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>Andres</t>
-  </si>
-  <si>
-    <t>Torres</t>
+    <t>Risso</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Enslow</t>
+  </si>
+  <si>
+    <t>Fats</t>
+  </si>
+  <si>
+    <t>Waller</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Aidan</t>
+  </si>
+  <si>
+    <t>Choi</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Testies</t>
   </si>
 </sst>
 </file>
@@ -406,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80685293-B585-495F-8E17-C24EE4395E9A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,16 +490,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
         <v>9</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>2000</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -453,13 +513,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2005</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -470,13 +530,211 @@
         <v>6</v>
       </c>
       <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
         <v>2003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>2001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.12 added cool stuff
</commit_message>
<xml_diff>
--- a/homies.xlsx
+++ b/homies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilen\Desktop\ANDRES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6205CF9B-5BB8-4356-9651-27C38AA9BC9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2A4E10-D4E0-47D7-998A-56CBA9E24E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="3315" windowWidth="21600" windowHeight="11385" xr2:uid="{BA09453C-118F-4BA7-BAAB-6338DA55BF77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Dylan</t>
   </si>
@@ -103,15 +103,6 @@
   </si>
   <si>
     <t>Alex</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Testies</t>
   </si>
 </sst>
 </file>
@@ -463,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80685293-B585-495F-8E17-C24EE4395E9A}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,13 +634,13 @@
         <v>18</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>1943</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,40 +692,6 @@
       </c>
       <c r="E14">
         <v>2003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>23</v>
-      </c>
-      <c r="E15">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16">
-        <v>23</v>
-      </c>
-      <c r="E16">
-        <v>2001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.16 made the code suck a little less now able to be put on github without exploding
</commit_message>
<xml_diff>
--- a/homies.xlsx
+++ b/homies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilen\Desktop\ANDRES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2A4E10-D4E0-47D7-998A-56CBA9E24E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B662CBD-AB9A-4443-BFA6-A70AB41BE7A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="3315" windowWidth="21600" windowHeight="11385" xr2:uid="{BA09453C-118F-4BA7-BAAB-6338DA55BF77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Dylan</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Provost</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>Edmond</t>
+  </si>
+  <si>
+    <t>Simonian</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80685293-B585-495F-8E17-C24EE4395E9A}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,15 +709,66 @@
         <v>2003</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17">
+        <v>2004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,26 +904,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5DED7A-C8C6-4DC9-89DC-29CE1AA1DB09}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8841B56B-CF78-4C33-90F2-6C4AE71BFA3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2eb21a81-502b-4e82-858d-b3e243ebbe07"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -881,9 +936,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8841B56B-CF78-4C33-90F2-6C4AE71BFA3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5DED7A-C8C6-4DC9-89DC-29CE1AA1DB09}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2eb21a81-502b-4e82-858d-b3e243ebbe07"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>